<commit_message>
Added few more test cases
</commit_message>
<xml_diff>
--- a/MarshTestCases.xlsx
+++ b/MarshTestCases.xlsx
@@ -706,7 +706,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1056,7 +1058,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Added customize and WR detailed view Test cases
</commit_message>
<xml_diff>
--- a/MarshTestCases.xlsx
+++ b/MarshTestCases.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Warranty_Upload" sheetId="2" r:id="rId1"/>
+    <sheet name="Record_Level_Validations" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="230">
   <si>
     <t>S.No</t>
   </si>
@@ -333,6 +333,597 @@
     <t>1.User should login into application with valid credentials.
 2.User should navigate to warranty upload page
 3.Verify desined upload page is matching with figma screens provided with all options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">warranty upload page should match with Figma screens provided
+2. The warranty page should have Header :   
+Header - 
+MARSH Logo and Client Logo on left side header.
+Language section dropdown and Logged User name and user role with Image. // Role is not available for now.
+Footer -
+2023 MARSH LLC. ALL RIGHT RESERVED
+Terms Of Use, Privacy Notices, FAQs </t>
+  </si>
+  <si>
+    <t>TC_WR_Upload_13</t>
+  </si>
+  <si>
+    <t>TC_WR_Upload_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">warranty upload page should match with Figma screens provided
+3.Menu on Warranty Page: 
+Page should have Warranty, Claim, Report Administration options
+4. Under warranty menu Page should display Warranty List -  "Upload Warranty " button and "Download Template"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">warranty upload page should match with Figma screens provided
+5. Warranty search with fields:  Created Pr for layout in mystique working on it
+Warranty Number, Application Number, VIN/Chassis, Warranty Start Date calendar, Warranty End Date calendar and Filter, Reset button and more filter option.    
+6. The Filter Menu with Status: Done
+All, Draft, Issued, Expired, Void, More as Dropdown with other status
+All - Active and all status policy should display under All.
+</t>
+  </si>
+  <si>
+    <t>TC_WR_Upload_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">warranty upload page should match with Figma screens provided.
+7. Options with Customize Column and Export to Excel. Done
+8. Header of the List view: Done( Headers selected as per figma)
+Warranty Number, Application Number, Status, Date Created, start and End Date, Duration, Car Module, Action, etc 
+Pagination    </t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_01</t>
+  </si>
+  <si>
+    <t>As a User working with excel data upload, I want the system to perform record level validation specifically for "Model Group" field to ensure accuracy and consistency.</t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has no model group  in uploaded file</t>
+  </si>
+  <si>
+    <t>1.Verify user is able to see error message ,if he try to upload the file which has no model group in it</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has no model group in it
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display an error message for records with missing Model Group entries.
+Error Message:
+   &lt;Error No&gt;Line : &lt;Line No&gt;, Missing mandatory [&lt;column name&gt;]
+</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_02</t>
+  </si>
+  <si>
+    <t>1.Verify user is able to see error message ,if he try to upload the file which has invalid model group in it</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has invalid model group in it
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display an error If does not exists in the car model master.
+Error Message: "&lt;Error No&gt; Line : &lt;Line No&gt;, Model doesn’t exist in Master Table : Model group[&lt;value&gt;] "
+</t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has invalid model group which does not exist in car model master table  in uploaded file</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_03</t>
+  </si>
+  <si>
+    <t>1.Verify user is able to see error message ,if he try to upload the file which has invalid model code in it</t>
+  </si>
+  <si>
+    <t>As a User working with excel data upload, I want the system to perform record level validation specifically for "Model Code" field to ensure accuracy and consistency.</t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has invalid model code which does not exist in car model master table  in uploaded file</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has no modelcode in it
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display an error message for records with missing Model Code entries.
+Error Message:
+   &lt;Error No&gt;Line : &lt;Line No&gt;, Missing mandatory [&lt;column name&gt;]
+</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_04</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_05</t>
+  </si>
+  <si>
+    <t>1.Verify user is able to see error message ,if he try to upload the file which has no model code in it</t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has no model code which does not exist in car model master table  in uploaded file</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has invalid  model code in it
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display an error If does not exists in the car model master.
+Error Message:
+&lt;Error No&gt; Line : &lt;Line No&gt;, Model doesn’t exist in Master Table : Model [&lt;value of model code&gt;]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_Record_Validation_06 </t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_07</t>
+  </si>
+  <si>
+    <t>1.Verify user is able to see error message ,if he try to upload the file which has no VIN number in it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a User working with vehicle data uploads, I want the system to perform record level validation specifically for the "VIN" (Vehicle Identification Number) filed to ensure accuracy and adherence to standards. </t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has no VIN number in it</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has no VIN number  in it
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display an error message for records with missing or empty "VIN" field.
+Error Message : &lt;Error No&gt; Line : &lt;Line No&gt;, Missing mandatory [&lt;Column Name&gt;]
+</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_08</t>
+  </si>
+  <si>
+    <t>1.Verify user is able to see error message ,if he tries to upload the file which has duplicate  VIN number in it</t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has same VIN number as existing records</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has same VIN number as existing records in it
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t>Display an error message If any this condition does not meet the error message should display.
+Error Message :  Error Message:  &lt;Error No&gt;Line : &lt;Line No&gt;, Duplicated data exist. : VIN [&lt;value&gt;]</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_09</t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has same VIN number as existing 
+Note :
+A record with the same VIN number is present in the the existing warranties with 
+status = "Registered"  AND  Warranty End        Date of that record &gt;= Warranty Start Date of the application</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has same VIN number as existing records in it
+Note: A record with the same VIN number is present in the the existing warranties with 
+status = "Registered"  AND  Warranty End        Date of that record &gt;= Warranty Start Date of the application
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Verify System is allowing user to upload VIN with alphanumeric characters </t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has same VIN number with alpha numeric characters excluding spaces ar both ends</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has same VIN number as alpha numeric
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t>System should allow user to upload a file with unique VIN number with alpha numeric characters</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a User managing upload data, I want the system to perform the record level validation specifically for the "Engine Number" and "Plate Number" fields to ensure accuracy and adherence to standards. </t>
+  </si>
+  <si>
+    <t>Display an error message for records with missing or empty Engine Number entries.
+Error Message:  &lt;Error No&gt;Line : &lt;Line No&gt;, Missing mandatory [&lt;column name&gt;]</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_12</t>
+  </si>
+  <si>
+    <t>1.Verify System is throwing error ,if user uploads file which has an empty plate number</t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has no  plate number in it</t>
+  </si>
+  <si>
+    <t>1.Verify System is throwing error ,if user uploads file which has an empty engine number</t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has no engine number   in it</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has no engine  in it
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has no plate number in it
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_13</t>
+  </si>
+  <si>
+    <t>As a User uploading file with data, I want the system to perform the record level validation specifically for the "Date of First Registration" fields to ensure accuracy and adherence to standards.</t>
+  </si>
+  <si>
+    <t>1.Verify System is throwing error ,if user uploads file which has an empty Date of first Registration.</t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has no  Date of First Registration.</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has no date of first registration in it
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t>Display an error message for records with missing or empty Date of First Registration entries.
+#TBD</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_14</t>
+  </si>
+  <si>
+    <t>1.Verify System is throwing error ,if user uploads file which has an invalid date format in  Date of first Registration data.</t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has invalid date format of   Date of First Registration.</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has invalid format of  date of first registration in it
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t>Provide an error message for entries with incorrect date formats.
+Error Message &lt;Error No&gt;Line : &lt;Line No&gt;, Missing mandatory [&lt;column name&gt;</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_15</t>
+  </si>
+  <si>
+    <t>1.Verify System is accepting warranty file ,if user uploads file which has an valid date format in  Date of first Registration data.</t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has valid date format of   Date of First Registration.</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has valid format( YYYY-MM-DD ) of  date of first registration in it
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_16</t>
+  </si>
+  <si>
+    <t>1.Verify System is throwing error ,if user uploads file which has an future date in Date of first Registration column.</t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has future date in Date of First Registration column.</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has future date in   date of first registration in it
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_17</t>
+  </si>
+  <si>
+    <t>1.Verify System is throwing error ,if user uploads file which has an past date in Date of first Registration column.</t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has past date in Date of First Registration column.</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has past date in   date of first registration in it
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t>Provide an error message for entries for records having past  date in date of first registration column
+#TBD</t>
+  </si>
+  <si>
+    <t>Provide an error message for entries for records having  future date in date of first registration column
+#TBD</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user excel data uploads for Vehicle price, I want the system to perform record level validation specifically for the "Vehicle Price" fields to ensure accuracy and adherence to standards. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Verify System is throwing error ,if user uploads file which has no data in vehicle price  field </t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has no data in vehicle price field</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has no data in vehicle price field
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display an error message for records with missing or empty Vehicle Price entries.
+Error Message : &lt;Error No&gt; Line : &lt;Line No&gt;, Missing mandatory [&lt;Column Name&gt;]
+</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Verify System is throwing error ,if user uploads file which has non numeric data in vehicle price  field </t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has non numeric data in vehicle price field</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has non numeric data in vehicle price field
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display an error message for records with invalid non numeric data entries
+#TBD
+</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Verify System is throwing error ,if user uploads file which has negetive value or decimal value  as a data in vehicle price  field </t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has negetive or decimal value as a data in vehicle price field</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has negetive or decimal value as a data in vehicle price field
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display an error message for records with negetive or decimal value  data entries
+#TBD
+</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Verify System is throwing error ,if user uploads file which has no data in vehicle type column </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a User managing upload data, I want the system to perform the record level validation to ensure that the combination of the "Product Code" and "Car Type" values exists in the product parameters, ensuring accuracy and valid data. </t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has no data in vehicle type field</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has no data in vehicle type field
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t>Display an error message for records with missing or empty Car Type entries.
+If value is missing then throw error message:
+Error Message: "&lt;Error No&gt; Line : &lt;Line No&gt;, Missing mandatory [&lt;Column Name&gt;]" 
+Car Type is an String type and its Mandatory field from file upload.</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_22</t>
+  </si>
+  <si>
+    <t>Display an error message for records with non-existent or invalid combination. 
+Error Message "&lt;Error No&gt; Line : &lt;Line No&gt;, Model doesn’t exist in Master Table : Car type [&lt;value&gt;]"</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_23</t>
+  </si>
+  <si>
+    <t>1.Verify System is throwing error ,if user uploads file which has invalid combination of car type and product code as a data and which does not exist  in Car master table</t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has  invalid  combination of product code and car type  in vehicle type field(Mismatched vehicle type and product code)</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has  invalid  combination of product code and car type which are mentioned in car master table  in vehicle type field.(Mismatched vehicle type and product code)
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t>User should upload a warranty which has  invalid  combination of product code and car type (Both car type and product code are invalid and random unknown values)</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has  invalid  combination of product code and car type(Both vehicle type and product code are invalid and random values)
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display an error message for records with invalid combination. 
+Error Message : "&lt;Error No&gt; Line : &lt;Line No&gt;, Invalid car type with product code : Vehicle Classification [&lt;value&gt;]" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Verify System is throwing error ,if user uploads file which has invalid combination of car type and product code as a data and which does not exist  in Car master table </t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Verify System is throwing error ,if user uploads file which has no data in millege column </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a User working with vehicle data uploads, I want the system to perform record level validation specifically for the "Current Mileage" filed to ensure accurate and plausible mileage information. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should upload a warranty which has no data in millege column </t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has  no data in millege column
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If value for current mileage is missing in uploaded file then throw error:
+&lt;Error No&gt; Line : &lt;Line No&gt;, Missing mandatory [&lt;Column Name&gt;]
+</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Verify System is throwing error ,if user uploads file which has non numeric or decimal value as a data in millege column </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If provided value for current mileage is non-numeric character or with decimal values then throw error:
+&lt;Error No&gt; Line : &lt;Line No&gt;, Invalid Data : Mileage [&lt;value&gt;]
+</t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has  non numeric or decimal value as a data in millege column
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Verify System is throwing error ,if user uploads file which has negetive  value as a data in millege column </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should upload a warranty which has negetive value as a data in millege column </t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has  negetive value as a data in millege column
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If provided value is less than 0 then throw error:
+&lt;Error No&gt; Line : &lt;Line No&gt;, Invalid Data : Mileage cannot be [&lt;value&gt;]
+</t>
+  </si>
+  <si>
+    <t>TC_Record_Validation_27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If Mileage is greater than maximum mileage from date of first registration then throw error:
+&lt;Error No&gt; Line : &lt;Line No&gt;, Present Mileage is not eligible for warranty enrolment : Mileage [&lt;value&gt;]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should upload a warranty which has value more than allowed limit in millege column as a data </t>
+  </si>
+  <si>
+    <t>1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page
+3.User should upload a warranty which has  a value exceeds maximum limit as a data in millege column
+4.verify user is able to see error message as per requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user inquiring about warranties, I want the ability to configure and view custom columns on the warranty page to tailor the displayed information according to my preferences. </t>
+  </si>
+  <si>
+    <t>User should be on warranty list page and has an access to option to customize the column selection on UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user  is able to to customize the order and preference of warranty list table columns </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page where he can see list of warranty which are all ready being uploaded till then 
+3.User clicks on customize column button from UI.
+4.Verify system is allowing user to change the order of selected  columns on his wish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User will see the cloumns what he selected will be displayed on warranty list table accordeing to his selection and order criteria </t>
+  </si>
+  <si>
+    <t>As User 
+I want to view the a warranty details on UI, 
+So that I can enter the related details and search the record.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user is able to see the details of choosen warranty from warranty list table </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be on warranty list table </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.user should login into application with valid credentials.
+2.User should navigate to warranty upload page where he can see list of warranty which are all ready being uploaded till then 
+3.User clicks on customize column button from UI.
+4.Verify system is allowing user to see the detailed view of warranty ,what he selected from the list </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User will see detailed view of warranty on UI ,once he clicks on corressponding warranty from list </t>
+  </si>
+  <si>
+    <t>TC_WR_Detailed_View_29</t>
+  </si>
+  <si>
+    <t>TC_Customize_Column_WR_List_28</t>
   </si>
 </sst>
 </file>
@@ -704,10 +1295,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1058,7 +1649,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1087,7 +1678,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1113,7 +1704,94 @@
         <v>20</v>
       </c>
       <c r="I13" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14">
+        <v>33262</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>79</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="288" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15">
+        <v>33262</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16">
+        <v>33262</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1123,12 +1801,940 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" customWidth="1"/>
+    <col min="6" max="6" width="23.88671875" customWidth="1"/>
+    <col min="7" max="7" width="35.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" customWidth="1"/>
+    <col min="9" max="9" width="27.44140625" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" customWidth="1"/>
+    <col min="12" max="12" width="13.21875" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2">
+        <v>34069</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3">
+        <v>34069</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>34069</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5">
+        <v>34071</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6">
+        <v>34071</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7">
+        <v>34071</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8">
+        <v>34072</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9">
+        <v>34072</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10">
+        <v>34072</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11">
+        <v>34072</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12">
+        <v>34073</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13">
+        <v>34073</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14">
+        <v>34074</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15">
+        <v>34074</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C16">
+        <v>34074</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17">
+        <v>34074</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C18">
+        <v>34074</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>167</v>
+      </c>
+      <c r="C19">
+        <v>33448</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20">
+        <v>33448</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21">
+        <v>33448</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>183</v>
+      </c>
+      <c r="C22">
+        <v>34076</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:10" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>189</v>
+      </c>
+      <c r="C23">
+        <v>34076</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>191</v>
+      </c>
+      <c r="C24">
+        <v>34076</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:10" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>199</v>
+      </c>
+      <c r="C25">
+        <v>34078</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>205</v>
+      </c>
+      <c r="C26">
+        <v>34078</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>209</v>
+      </c>
+      <c r="C27">
+        <v>34078</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>214</v>
+      </c>
+      <c r="C28">
+        <v>34078</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>229</v>
+      </c>
+      <c r="C29">
+        <v>36061</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>228</v>
+      </c>
+      <c r="C30">
+        <v>34669</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>